<commit_message>
updates to final v2.0 on edi
</commit_message>
<xml_diff>
--- a/data-raw/metadata/F4F2021_ContinuousTempDO_AttributesTable.xlsx
+++ b/data-raw/metadata/F4F2021_ContinuousTempDO_AttributesTable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacobshikora\Documents\CalTrout\BORCharter\DataTransfer\2021Submission\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\data-stewardship\EDI_data_repos_to_upload\fish-food-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCCC9AF-7FD4-40AD-A51F-F8D15734F0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232A048F-4686-44C3-8442-CDCC8722F8B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{17824303-BC38-4FFE-852F-26E788E3CF6F}"/>
   </bookViews>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -144,7 +142,7 @@
     <t>fahrenheit</t>
   </si>
   <si>
-    <t>mm/dd/yyyy hh:mm</t>
+    <t>yyyy-mm-dd hh:mm:ss</t>
   </si>
 </sst>
 </file>
@@ -503,7 +501,7 @@
   <dimension ref="A1:AMJ8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>